<commit_message>
QR and Hessenberg decomposition, and test
</commit_message>
<xml_diff>
--- a/jacobi/src/test/resources/jacobi/test/data/QRDecompTest.xlsx
+++ b/jacobi/src/test/resources/jacobi/test/data/QRDecompTest.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="4x4" sheetId="1" r:id="rId1"/>
     <sheet name="6x6" sheetId="2" r:id="rId2"/>
     <sheet name="9x3" sheetId="4" r:id="rId3"/>
-    <sheet name="rand" sheetId="3" r:id="rId4"/>
+    <sheet name="Degen 8x3" sheetId="5" r:id="rId4"/>
+    <sheet name="rand" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="12">
   <si>
     <t>#1</t>
   </si>
@@ -50,6 +51,9 @@
   </si>
   <si>
     <t>#5</t>
+  </si>
+  <si>
+    <t>Householder</t>
   </si>
 </sst>
 </file>
@@ -1245,7 +1249,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A48" sqref="A48:E52"/>
     </sheetView>
   </sheetViews>
@@ -3659,8 +3663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC47"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:C47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6167,10 +6171,1457 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>12.832681232845054</v>
+      </c>
+      <c r="B3">
+        <f>A3</f>
+        <v>12.832681232845054</v>
+      </c>
+      <c r="C3">
+        <v>-17.144650356428635</v>
+      </c>
+      <c r="E3">
+        <f>A3</f>
+        <v>12.832681232845054</v>
+      </c>
+      <c r="F3">
+        <f>SQRT(SUMPRODUCT(E3:E10,E3:E10))</f>
+        <v>40.80706333490032</v>
+      </c>
+      <c r="G3">
+        <f>E3+F3</f>
+        <v>53.639744567745375</v>
+      </c>
+      <c r="H3">
+        <f>SQRT(SUMPRODUCT(G3:G10,G3:G10))</f>
+        <v>66.164649985379057</v>
+      </c>
+      <c r="I3">
+        <f>G3/H$3</f>
+        <v>0.81070094951909499</v>
+      </c>
+      <c r="K3">
+        <f t="array" ref="K3:R10">MMULT(I3:I10,TRANSPOSE(I3:I10))</f>
+        <v>0.65723602955116223</v>
+      </c>
+      <c r="L3">
+        <v>6.5830764327154623E-2</v>
+      </c>
+      <c r="M3">
+        <v>0.14673621764819494</v>
+      </c>
+      <c r="N3">
+        <v>9.5177956310034187E-2</v>
+      </c>
+      <c r="O3">
+        <v>0.30434310046074525</v>
+      </c>
+      <c r="P3">
+        <v>0.22138174048057704</v>
+      </c>
+      <c r="Q3">
+        <v>-9.4550445593212119E-3</v>
+      </c>
+      <c r="R3">
+        <v>-0.22051935257058056</v>
+      </c>
+      <c r="T3">
+        <f>1-2*K3</f>
+        <v>-0.31447205910232445</v>
+      </c>
+      <c r="U3">
+        <f t="shared" ref="U3:AA3" si="0">-2*L3</f>
+        <v>-0.13166152865430925</v>
+      </c>
+      <c r="V3">
+        <f t="shared" si="0"/>
+        <v>-0.29347243529638989</v>
+      </c>
+      <c r="W3">
+        <f t="shared" si="0"/>
+        <v>-0.19035591262006837</v>
+      </c>
+      <c r="X3">
+        <f t="shared" si="0"/>
+        <v>-0.60868620092149051</v>
+      </c>
+      <c r="Y3">
+        <f t="shared" si="0"/>
+        <v>-0.44276348096115409</v>
+      </c>
+      <c r="Z3">
+        <f t="shared" si="0"/>
+        <v>1.8910089118642424E-2</v>
+      </c>
+      <c r="AA3">
+        <f t="shared" si="0"/>
+        <v>0.44103870514116111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5.3727203385661895</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:B10" si="1">A4</f>
+        <v>5.3727203385661895</v>
+      </c>
+      <c r="C4">
+        <v>-4.8811427524532647</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E10" si="2">A4</f>
+        <v>5.3727203385661895</v>
+      </c>
+      <c r="G4">
+        <f>E4</f>
+        <v>5.3727203385661895</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I10" si="3">G4/H$3</f>
+        <v>8.1202278554385818E-2</v>
+      </c>
+      <c r="K4">
+        <v>6.5830764327154623E-2</v>
+      </c>
+      <c r="L4">
+        <v>6.5938100424240672E-3</v>
+      </c>
+      <c r="M4">
+        <v>1.469754689019895E-2</v>
+      </c>
+      <c r="N4">
+        <v>9.5333142573832894E-3</v>
+      </c>
+      <c r="O4">
+        <v>3.0483932742867439E-2</v>
+      </c>
+      <c r="P4">
+        <v>2.2174270016610053E-2</v>
+      </c>
+      <c r="Q4">
+        <v>-9.4704608709977498E-4</v>
+      </c>
+      <c r="R4">
+        <v>-2.2087890614524722E-2</v>
+      </c>
+      <c r="T4">
+        <f t="shared" ref="T4:T10" si="4">-2*K4</f>
+        <v>-0.13166152865430925</v>
+      </c>
+      <c r="U4">
+        <f>1-2*L4</f>
+        <v>0.98681237991515192</v>
+      </c>
+      <c r="V4">
+        <f t="shared" ref="V4:V10" si="5">-2*M4</f>
+        <v>-2.93950937803979E-2</v>
+      </c>
+      <c r="W4">
+        <f t="shared" ref="W4:W10" si="6">-2*N4</f>
+        <v>-1.9066628514766579E-2</v>
+      </c>
+      <c r="X4">
+        <f t="shared" ref="X4:X10" si="7">-2*O4</f>
+        <v>-6.0967865485734879E-2</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" ref="Y4:Y10" si="8">-2*P4</f>
+        <v>-4.4348540033220106E-2</v>
+      </c>
+      <c r="Z4">
+        <f t="shared" ref="Z4:Z10" si="9">-2*Q4</f>
+        <v>1.89409217419955E-3</v>
+      </c>
+      <c r="AA4">
+        <f t="shared" ref="AA4:AA10" si="10">-2*R4</f>
+        <v>4.4175781229049443E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>11.975748254187216</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="1"/>
+        <v>11.975748254187216</v>
+      </c>
+      <c r="C5">
+        <v>-2.0862583502972534</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>11.975748254187216</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G10" si="11">E5</f>
+        <v>11.975748254187216</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="3"/>
+        <v>0.18099919302578635</v>
+      </c>
+      <c r="K5">
+        <v>0.14673621764819494</v>
+      </c>
+      <c r="L5">
+        <v>1.469754689019895E-2</v>
+      </c>
+      <c r="M5">
+        <v>3.2760707875985867E-2</v>
+      </c>
+      <c r="N5">
+        <v>2.1249676956933149E-2</v>
+      </c>
+      <c r="O5">
+        <v>6.7948428602479696E-2</v>
+      </c>
+      <c r="P5">
+        <v>4.9426260572900324E-2</v>
+      </c>
+      <c r="Q5">
+        <v>-2.1109577289568503E-3</v>
+      </c>
+      <c r="R5">
+        <v>-4.923372161525244E-2</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="4"/>
+        <v>-0.29347243529638989</v>
+      </c>
+      <c r="U5">
+        <f t="shared" ref="U4:U10" si="12">-2*L5</f>
+        <v>-2.93950937803979E-2</v>
+      </c>
+      <c r="V5">
+        <f>1-2*M5</f>
+        <v>0.93447858424802832</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="6"/>
+        <v>-4.2499353913866299E-2</v>
+      </c>
+      <c r="X5">
+        <f t="shared" si="7"/>
+        <v>-0.13589685720495939</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" si="8"/>
+        <v>-9.8852521145800648E-2</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" si="9"/>
+        <v>4.2219154579137006E-3</v>
+      </c>
+      <c r="AA5">
+        <f t="shared" si="10"/>
+        <v>9.8467443230504881E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>7.7678657824598787</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="1"/>
+        <v>7.7678657824598787</v>
+      </c>
+      <c r="C6">
+        <v>22.110470108929739</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>7.7678657824598787</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="11"/>
+        <v>7.7678657824598787</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="3"/>
+        <v>0.11740205357659124</v>
+      </c>
+      <c r="K6">
+        <v>9.5177956310034187E-2</v>
+      </c>
+      <c r="L6">
+        <v>9.5333142573832894E-3</v>
+      </c>
+      <c r="M6">
+        <v>2.1249676956933149E-2</v>
+      </c>
+      <c r="N6">
+        <v>1.37832421840008E-2</v>
+      </c>
+      <c r="O6">
+        <v>4.40735945938555E-2</v>
+      </c>
+      <c r="P6">
+        <v>3.2059504768308586E-2</v>
+      </c>
+      <c r="Q6">
+        <v>-1.3692368913357745E-3</v>
+      </c>
+      <c r="R6">
+        <v>-3.1934617642330416E-2</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="4"/>
+        <v>-0.19035591262006837</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="12"/>
+        <v>-1.9066628514766579E-2</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="5"/>
+        <v>-4.2499353913866299E-2</v>
+      </c>
+      <c r="W6">
+        <f>1-2*N6</f>
+        <v>0.97243351563199842</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="7"/>
+        <v>-8.8147189187711E-2</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" si="8"/>
+        <v>-6.4119009536617172E-2</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" si="9"/>
+        <v>2.738473782671549E-3</v>
+      </c>
+      <c r="AA6">
+        <f t="shared" si="10"/>
+        <v>6.3869235284660833E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>24.838696352083119</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="1"/>
+        <v>24.838696352083119</v>
+      </c>
+      <c r="C7">
+        <v>12.761744712530202</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>24.838696352083119</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="11"/>
+        <v>24.838696352083119</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="3"/>
+        <v>0.37540735661069663</v>
+      </c>
+      <c r="K7">
+        <v>0.30434310046074525</v>
+      </c>
+      <c r="L7">
+        <v>3.0483932742867439E-2</v>
+      </c>
+      <c r="M7">
+        <v>6.7948428602479696E-2</v>
+      </c>
+      <c r="N7">
+        <v>4.40735945938555E-2</v>
+      </c>
+      <c r="O7">
+        <v>0.14093068339743076</v>
+      </c>
+      <c r="P7">
+        <v>0.1025141688127888</v>
+      </c>
+      <c r="Q7">
+        <v>-4.3783016249785717E-3</v>
+      </c>
+      <c r="R7">
+        <v>-0.10211482702608331</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="4"/>
+        <v>-0.60868620092149051</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="12"/>
+        <v>-6.0967865485734879E-2</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="5"/>
+        <v>-0.13589685720495939</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="6"/>
+        <v>-8.8147189187711E-2</v>
+      </c>
+      <c r="X7">
+        <f>1-2*O7</f>
+        <v>0.71813863320513849</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" si="8"/>
+        <v>-0.20502833762557759</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" si="9"/>
+        <v>8.7566032499571435E-3</v>
+      </c>
+      <c r="AA7">
+        <f t="shared" si="10"/>
+        <v>0.20422965405216661</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>18.06787740996274</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="1"/>
+        <v>18.06787740996274</v>
+      </c>
+      <c r="C8">
+        <v>19.123227480634199</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>18.06787740996274</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="11"/>
+        <v>18.06787740996274</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>0.27307448031472015</v>
+      </c>
+      <c r="K8">
+        <v>0.22138174048057704</v>
+      </c>
+      <c r="L8">
+        <v>2.2174270016610053E-2</v>
+      </c>
+      <c r="M8">
+        <v>4.9426260572900324E-2</v>
+      </c>
+      <c r="N8">
+        <v>3.2059504768308586E-2</v>
+      </c>
+      <c r="O8">
+        <v>0.1025141688127888</v>
+      </c>
+      <c r="P8">
+        <v>7.4569671799154483E-2</v>
+      </c>
+      <c r="Q8">
+        <v>-3.1848135627826199E-3</v>
+      </c>
+      <c r="R8">
+        <v>-7.427918721233899E-2</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="4"/>
+        <v>-0.44276348096115409</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="12"/>
+        <v>-4.4348540033220106E-2</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="5"/>
+        <v>-9.8852521145800648E-2</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="6"/>
+        <v>-6.4119009536617172E-2</v>
+      </c>
+      <c r="X8">
+        <f t="shared" si="7"/>
+        <v>-0.20502833762557759</v>
+      </c>
+      <c r="Y8">
+        <f>1-2*P8</f>
+        <v>0.85086065640169106</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="9"/>
+        <v>6.3696271255652397E-3</v>
+      </c>
+      <c r="AA8">
+        <f t="shared" si="10"/>
+        <v>0.14855837442467798</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>-0.77166520433305053</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="1"/>
+        <v>-0.77166520433305053</v>
+      </c>
+      <c r="C9">
+        <v>15.953500007153757</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>-0.77166520433305053</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="11"/>
+        <v>-0.77166520433305053</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>-1.1662801881421147E-2</v>
+      </c>
+      <c r="K9">
+        <v>-9.4550445593212119E-3</v>
+      </c>
+      <c r="L9">
+        <v>-9.4704608709977498E-4</v>
+      </c>
+      <c r="M9">
+        <v>-2.1109577289568503E-3</v>
+      </c>
+      <c r="N9">
+        <v>-1.3692368913357745E-3</v>
+      </c>
+      <c r="O9">
+        <v>-4.3783016249785717E-3</v>
+      </c>
+      <c r="P9">
+        <v>-3.1848135627826199E-3</v>
+      </c>
+      <c r="Q9">
+        <v>1.3602094772528065E-4</v>
+      </c>
+      <c r="R9">
+        <v>3.1724071885885501E-3</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="4"/>
+        <v>1.8910089118642424E-2</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="12"/>
+        <v>1.89409217419955E-3</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="5"/>
+        <v>4.2219154579137006E-3</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="6"/>
+        <v>2.738473782671549E-3</v>
+      </c>
+      <c r="X9">
+        <f t="shared" si="7"/>
+        <v>8.7566032499571435E-3</v>
+      </c>
+      <c r="Y9">
+        <f t="shared" si="8"/>
+        <v>6.3696271255652397E-3</v>
+      </c>
+      <c r="Z9">
+        <f>1-2*Q9</f>
+        <v>0.9997279581045494</v>
+      </c>
+      <c r="AA9">
+        <f t="shared" si="10"/>
+        <v>-6.3448143771771002E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>-17.997494373837785</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="1"/>
+        <v>-17.997494373837785</v>
+      </c>
+      <c r="C10">
+        <v>2.7787734711408056</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>-17.997494373837785</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="11"/>
+        <v>-17.997494373837785</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="3"/>
+        <v>-0.2720107244248226</v>
+      </c>
+      <c r="K10">
+        <v>-0.22051935257058056</v>
+      </c>
+      <c r="L10">
+        <v>-2.2087890614524722E-2</v>
+      </c>
+      <c r="M10">
+        <v>-4.923372161525244E-2</v>
+      </c>
+      <c r="N10">
+        <v>-3.1934617642330416E-2</v>
+      </c>
+      <c r="O10">
+        <v>-0.10211482702608331</v>
+      </c>
+      <c r="P10">
+        <v>-7.427918721233899E-2</v>
+      </c>
+      <c r="Q10">
+        <v>3.1724071885885501E-3</v>
+      </c>
+      <c r="R10">
+        <v>7.3989834202116786E-2</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="4"/>
+        <v>0.44103870514116111</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="12"/>
+        <v>4.4175781229049443E-2</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="5"/>
+        <v>9.8467443230504881E-2</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="6"/>
+        <v>6.3869235284660833E-2</v>
+      </c>
+      <c r="X10">
+        <f t="shared" si="7"/>
+        <v>0.20422965405216661</v>
+      </c>
+      <c r="Y10">
+        <f t="shared" si="8"/>
+        <v>0.14855837442467798</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" si="9"/>
+        <v>-6.3448143771771002E-3</v>
+      </c>
+      <c r="AA10">
+        <f>1-2*R10</f>
+        <v>0.8520203315957664</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="array" ref="A14:C21">MMULT(T3:AA10,A3:C10)</f>
+        <v>-40.807063334900327</v>
+      </c>
+      <c r="B14">
+        <v>-40.807063334900327</v>
+      </c>
+      <c r="C14">
+        <v>-12.270163093036922</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <f t="array" ref="K14:R21">MMULT(I14:I21,TRANSPOSE(I14:I21))</f>
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <f>1-2*K14</f>
+        <v>1</v>
+      </c>
+      <c r="U14">
+        <f t="shared" ref="U14" si="13">-2*L14</f>
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <f t="shared" ref="V14:V15" si="14">-2*M14</f>
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <f t="shared" ref="W14:W16" si="15">-2*N14</f>
+        <v>0</v>
+      </c>
+      <c r="X14">
+        <f t="shared" ref="X14:X17" si="16">-2*O14</f>
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <f t="shared" ref="Y14:Y18" si="17">-2*P14</f>
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <f t="shared" ref="Z14:Z19" si="18">-2*Q14</f>
+        <v>0</v>
+      </c>
+      <c r="AA14">
+        <f t="shared" ref="AA14:AA20" si="19">-2*R14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>-1.1102230246251565E-15</v>
+      </c>
+      <c r="B15">
+        <v>-1.1102230246251565E-15</v>
+      </c>
+      <c r="C15">
+        <v>-4.3928992481049134</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <f t="shared" ref="T15:T21" si="20">-2*K15</f>
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <f>1-2*L15</f>
+        <v>1</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>-8.8817841970012523E-16</v>
+      </c>
+      <c r="B16">
+        <v>-8.8817841970012523E-16</v>
+      </c>
+      <c r="C16">
+        <v>-0.99796770303485904</v>
+      </c>
+      <c r="E16">
+        <f>C16</f>
+        <v>-0.99796770303485904</v>
+      </c>
+      <c r="F16">
+        <f>SQRT(SUMPRODUCT(E16:E21,E16:E21))</f>
+        <v>37.840866645577719</v>
+      </c>
+      <c r="G16">
+        <f>E16-F16</f>
+        <v>-38.838834348612579</v>
+      </c>
+      <c r="H16">
+        <f>SQRT(SUMPRODUCT(G16:G21,G16:G21))</f>
+        <v>54.216144297718778</v>
+      </c>
+      <c r="I16">
+        <f>G16/H$16</f>
+        <v>-0.7163702777411779</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0.5131863748309724</v>
+      </c>
+      <c r="N16">
+        <v>-0.30147791769844307</v>
+      </c>
+      <c r="O16">
+        <v>-0.19844880969418294</v>
+      </c>
+      <c r="P16">
+        <v>-0.27437449800083219</v>
+      </c>
+      <c r="Q16">
+        <v>-0.20987065958719431</v>
+      </c>
+      <c r="R16">
+        <v>-1.5106147133439817E-2</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <f t="shared" ref="U16:U21" si="21">-2*L16</f>
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <f>1-2*M16</f>
+        <v>-2.6372749661944805E-2</v>
+      </c>
+      <c r="W16">
+        <f t="shared" si="15"/>
+        <v>0.60295583539688613</v>
+      </c>
+      <c r="X16">
+        <f t="shared" si="16"/>
+        <v>0.39689761938836587</v>
+      </c>
+      <c r="Y16">
+        <f t="shared" si="17"/>
+        <v>0.54874899600166438</v>
+      </c>
+      <c r="Z16">
+        <f t="shared" si="18"/>
+        <v>0.41974131917438862</v>
+      </c>
+      <c r="AA16">
+        <f t="shared" si="19"/>
+        <v>3.0212294266879634E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>-8.8817841970012523E-16</v>
+      </c>
+      <c r="B17">
+        <v>-8.8817841970012523E-16</v>
+      </c>
+      <c r="C17">
+        <v>22.81637136042648</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ref="E17:E21" si="22">C17</f>
+        <v>22.81637136042648</v>
+      </c>
+      <c r="G17">
+        <f>E17</f>
+        <v>22.81637136042648</v>
+      </c>
+      <c r="I17">
+        <f t="shared" ref="I17:I21" si="23">G17/H$16</f>
+        <v>0.42084090737132174</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>-0.30147791769844307</v>
+      </c>
+      <c r="N17">
+        <v>0.17710706931711739</v>
+      </c>
+      <c r="O17">
+        <v>0.1165812984338143</v>
+      </c>
+      <c r="P17">
+        <v>0.16118481780443061</v>
+      </c>
+      <c r="Q17">
+        <v>0.12329121064288925</v>
+      </c>
+      <c r="R17">
+        <v>8.8742998754316946E-3</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <f t="shared" ref="V17:V21" si="24">-2*M17</f>
+        <v>0.60295583539688613</v>
+      </c>
+      <c r="W17">
+        <f>1-2*N17</f>
+        <v>0.64578586136576521</v>
+      </c>
+      <c r="X17">
+        <f t="shared" si="16"/>
+        <v>-0.23316259686762861</v>
+      </c>
+      <c r="Y17">
+        <f t="shared" si="17"/>
+        <v>-0.32236963560886123</v>
+      </c>
+      <c r="Z17">
+        <f t="shared" si="18"/>
+        <v>-0.24658242128577851</v>
+      </c>
+      <c r="AA17">
+        <f t="shared" si="19"/>
+        <v>-1.7748599750863389E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>-5.773159728050814E-15</v>
+      </c>
+      <c r="B18">
+        <v>-5.773159728050814E-15</v>
+      </c>
+      <c r="C18">
+        <v>15.018949887222417</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="22"/>
+        <v>15.018949887222417</v>
+      </c>
+      <c r="G18">
+        <f t="shared" ref="G18:G21" si="25">E18</f>
+        <v>15.018949887222417</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="23"/>
+        <v>0.27701988184088483</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>-0.19844880969418294</v>
+      </c>
+      <c r="N18">
+        <v>0.1165812984338143</v>
+      </c>
+      <c r="O18">
+        <v>7.6740014935137796E-2</v>
+      </c>
+      <c r="P18">
+        <v>0.10610042512652061</v>
+      </c>
+      <c r="Q18">
+        <v>8.1156836244004965E-2</v>
+      </c>
+      <c r="R18">
+        <v>5.8415364567769492E-3</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <f t="shared" si="24"/>
+        <v>0.39689761938836587</v>
+      </c>
+      <c r="W18">
+        <f t="shared" ref="W18:W21" si="26">-2*N18</f>
+        <v>-0.23316259686762861</v>
+      </c>
+      <c r="X18">
+        <f>1-2*O18</f>
+        <v>0.84651997012972435</v>
+      </c>
+      <c r="Y18">
+        <f t="shared" si="17"/>
+        <v>-0.21220085025304122</v>
+      </c>
+      <c r="Z18">
+        <f t="shared" si="18"/>
+        <v>-0.16231367248800993</v>
+      </c>
+      <c r="AA18">
+        <f t="shared" si="19"/>
+        <v>-1.1683072913553898E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>-5.3290705182007514E-15</v>
+      </c>
+      <c r="B19">
+        <v>-5.3290705182007514E-15</v>
+      </c>
+      <c r="C19">
+        <v>20.765137579593645</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="22"/>
+        <v>20.765137579593645</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="25"/>
+        <v>20.765137579593645</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="23"/>
+        <v>0.38300653520407885</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>-0.27437449800083219</v>
+      </c>
+      <c r="N19">
+        <v>0.16118481780443061</v>
+      </c>
+      <c r="O19">
+        <v>0.10610042512652061</v>
+      </c>
+      <c r="P19">
+        <v>0.14669400600903329</v>
+      </c>
+      <c r="Q19">
+        <v>0.11220710387781843</v>
+      </c>
+      <c r="R19">
+        <v>8.0764839827039622E-3</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <f t="shared" si="24"/>
+        <v>0.54874899600166438</v>
+      </c>
+      <c r="W19">
+        <f t="shared" si="26"/>
+        <v>-0.32236963560886123</v>
+      </c>
+      <c r="X19">
+        <f t="shared" ref="X19:X21" si="27">-2*O19</f>
+        <v>-0.21220085025304122</v>
+      </c>
+      <c r="Y19">
+        <f>1-2*P19</f>
+        <v>0.70661198798193348</v>
+      </c>
+      <c r="Z19">
+        <f t="shared" si="18"/>
+        <v>-0.22441420775563686</v>
+      </c>
+      <c r="AA19">
+        <f t="shared" si="19"/>
+        <v>-1.6152967965407924E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1.6653345369377348E-16</v>
+      </c>
+      <c r="B20">
+        <v>1.6653345369377348E-16</v>
+      </c>
+      <c r="C20">
+        <v>15.883375284516918</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="22"/>
+        <v>15.883375284516918</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="25"/>
+        <v>15.883375284516918</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="23"/>
+        <v>0.29296394072761889</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>-0.20987065958719431</v>
+      </c>
+      <c r="N20">
+        <v>0.12329121064288925</v>
+      </c>
+      <c r="O20">
+        <v>8.1156836244004965E-2</v>
+      </c>
+      <c r="P20">
+        <v>0.11220710387781843</v>
+      </c>
+      <c r="Q20">
+        <v>8.5827870566655792E-2</v>
+      </c>
+      <c r="R20">
+        <v>6.1777498745176733E-3</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <f t="shared" si="24"/>
+        <v>0.41974131917438862</v>
+      </c>
+      <c r="W20">
+        <f t="shared" si="26"/>
+        <v>-0.24658242128577851</v>
+      </c>
+      <c r="X20">
+        <f t="shared" si="27"/>
+        <v>-0.16231367248800993</v>
+      </c>
+      <c r="Y20">
+        <f t="shared" ref="Y20:Y21" si="28">-2*P20</f>
+        <v>-0.22441420775563686</v>
+      </c>
+      <c r="Z20">
+        <f>1-2*Q20</f>
+        <v>0.82834425886668839</v>
+      </c>
+      <c r="AA20">
+        <f t="shared" si="19"/>
+        <v>-1.2355499749035347E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>5.3290705182007514E-15</v>
+      </c>
+      <c r="B21">
+        <v>5.3290705182007514E-15</v>
+      </c>
+      <c r="C21">
+        <v>1.1432593984099446</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="22"/>
+        <v>1.1432593984099446</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="25"/>
+        <v>1.1432593984099446</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="23"/>
+        <v>2.108706572957179E-2</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>-1.5106147133439817E-2</v>
+      </c>
+      <c r="N21">
+        <v>8.8742998754316946E-3</v>
+      </c>
+      <c r="O21">
+        <v>5.8415364567769492E-3</v>
+      </c>
+      <c r="P21">
+        <v>8.0764839827039622E-3</v>
+      </c>
+      <c r="Q21">
+        <v>6.1777498745176733E-3</v>
+      </c>
+      <c r="R21">
+        <v>4.4466434108328108E-4</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <f t="shared" si="24"/>
+        <v>3.0212294266879634E-2</v>
+      </c>
+      <c r="W21">
+        <f t="shared" si="26"/>
+        <v>-1.7748599750863389E-2</v>
+      </c>
+      <c r="X21">
+        <f t="shared" si="27"/>
+        <v>-1.1683072913553898E-2</v>
+      </c>
+      <c r="Y21">
+        <f t="shared" si="28"/>
+        <v>-1.6152967965407924E-2</v>
+      </c>
+      <c r="Z21">
+        <f t="shared" ref="Z21" si="29">-2*Q21</f>
+        <v>-1.2355499749035347E-2</v>
+      </c>
+      <c r="AA21">
+        <f>1-2*R21</f>
+        <v>0.99911067131783349</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="array" ref="A25:C32">MMULT(T14:AA21,A14:C21)</f>
+        <v>-40.807063334900327</v>
+      </c>
+      <c r="B25">
+        <v>-40.807063334900327</v>
+      </c>
+      <c r="C25">
+        <v>-12.270163093036922</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>-1.1102230246251565E-15</v>
+      </c>
+      <c r="B26">
+        <v>-1.1102230246251565E-15</v>
+      </c>
+      <c r="C26">
+        <v>-4.3928992481049134</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>-5.4968796846058428E-15</v>
+      </c>
+      <c r="B27">
+        <v>-5.4968796846058428E-15</v>
+      </c>
+      <c r="C27">
+        <v>37.840866645577719</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1.8192622466573718E-15</v>
+      </c>
+      <c r="B28">
+        <v>1.8192622466573718E-15</v>
+      </c>
+      <c r="C28">
+        <v>2.8206603719382883E-15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>-3.9909781949618794E-15</v>
+      </c>
+      <c r="B29">
+        <v>-3.9909781949618794E-15</v>
+      </c>
+      <c r="C29">
+        <v>1.6861512186494565E-15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>-2.8650337510305462E-15</v>
+      </c>
+      <c r="B30">
+        <v>-2.8650337510305462E-15</v>
+      </c>
+      <c r="C30">
+        <v>1.9463597400459776E-15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2.0512896002782876E-15</v>
+      </c>
+      <c r="B31">
+        <v>2.0512896002782876E-15</v>
+      </c>
+      <c r="C31">
+        <v>1.609823385706477E-15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>5.4647321858057555E-15</v>
+      </c>
+      <c r="B32">
+        <v>5.4647321858057555E-15</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:D13"/>
+      <selection activeCell="C5" sqref="C5:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6178,1021 +7629,1021 @@
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1">
         <f ca="1">50*RAND()-25</f>
-        <v>15.308224611761403</v>
+        <v>1.8436622307579462</v>
       </c>
       <c r="B1">
         <f t="shared" ref="B1:H16" ca="1" si="0">50*RAND()-25</f>
-        <v>22.984133998297075</v>
+        <v>11.257841458605292</v>
       </c>
       <c r="C1">
         <f t="shared" ca="1" si="0"/>
-        <v>21.84343017875603</v>
+        <v>4.239566844320052</v>
       </c>
       <c r="D1">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.8567254935900763</v>
+        <v>-20.705904248728519</v>
       </c>
       <c r="E1">
         <f t="shared" ca="1" si="0"/>
-        <v>10.9057534969957</v>
+        <v>11.137464630272845</v>
       </c>
       <c r="F1">
         <f t="shared" ca="1" si="0"/>
-        <v>22.802448168595909</v>
+        <v>6.2095199912570074</v>
       </c>
       <c r="G1">
         <f t="shared" ca="1" si="0"/>
-        <v>-9.4269620263939427</v>
+        <v>24.742231745824661</v>
       </c>
       <c r="H1">
         <f t="shared" ca="1" si="0"/>
-        <v>-23.160531639755344</v>
+        <v>16.691227475745656</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:H30" ca="1" si="1">50*RAND()-25</f>
-        <v>24.207902149581905</v>
+        <v>-9.8616044699600778</v>
       </c>
       <c r="B2">
         <f t="shared" ca="1" si="0"/>
-        <v>-7.6721234257732576</v>
+        <v>-17.944357528026515</v>
       </c>
       <c r="C2">
         <f t="shared" ca="1" si="0"/>
-        <v>23.290698540481422</v>
+        <v>-4.2050839323885931</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.4054911922381521</v>
+        <v>-6.8412058351196521</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>-17.700765809607745</v>
+        <v>-21.865448599013853</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>16.321389061276115</v>
+        <v>-4.4537631392773598</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.2484626546566346</v>
+        <v>8.3197656303904495</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>-12.367620167683102</v>
+        <v>6.517947368829546</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ca="1" si="1"/>
-        <v>-12.86981844643525</v>
+        <v>-17.159291928496089</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.4749568972782683</v>
+        <v>7.9315706410946163</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>-20.979750816760124</v>
+        <v>4.4834947317439706</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>14.471963631800385</v>
+        <v>22.831305171178492</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>-21.063388964069048</v>
+        <v>-8.2295573884637108</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>-21.89080042262918</v>
+        <v>-11.427545950050543</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="0"/>
-        <v>21.580957747662254</v>
+        <v>18.464697813982276</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="0"/>
-        <v>-20.646671200934364</v>
+        <v>-17.666152003826411</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="1"/>
-        <v>4.1083589212718081</v>
+        <v>-16.172579076709866</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.2247484091223875</v>
+        <v>-3.3769851686092309</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>9.6397450005120291</v>
+        <v>-17.548181236617378</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>16.185665451574131</v>
+        <v>-12.33653989420112</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>2.105710899561636</v>
+        <v>-4.7971019063078053</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.7557480256106217</v>
+        <v>-17.963485055206796</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>11.445673979188456</v>
+        <v>-6.9798059937726933</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.8386423435257555</v>
+        <v>9.1334426393971029</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="1"/>
-        <v>9.8430671034582531</v>
+        <v>-0.11171424629897686</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>21.25258896543987</v>
+        <v>3.7759821436399399</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.57933916864836732</v>
+        <v>-2.9759454123956459</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>16.577484019985143</v>
+        <v>14.2800333155757</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.98898077406329321</v>
+        <v>-11.82725884150469</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>19.836602786445305</v>
+        <v>8.6591963828579708</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>20.471245067729207</v>
+        <v>24.818062166537047</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>-20.357600327367464</v>
+        <v>-21.098997874399682</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="1"/>
-        <v>12.890489181224758</v>
+        <v>-23.28779517517065</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>11.517092649364393</v>
+        <v>-4.7249053640952177</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.0773993345194306</v>
+        <v>-0.79887587048206754</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>-11.303163706045011</v>
+        <v>-23.582891930658707</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>21.025119258328118</v>
+        <v>3.0020607758819473</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>20.934123461671085</v>
+        <v>-14.971035161249047</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>-19.116466104214581</v>
+        <v>9.6679569606653502</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>-17.720826493597002</v>
+        <v>16.030835975824395</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="1"/>
-        <v>-21.034652431281202</v>
+        <v>-17.470503180972297</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>-11.790599820002463</v>
+        <v>0.22022494717863239</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>10.06469677622789</v>
+        <v>-6.960824873114678</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.1345875270875432</v>
+        <v>-3.3385076157908813</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>16.120373267681224</v>
+        <v>15.973840247502885</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>-19.09514954735431</v>
+        <v>-5.9033617894554915</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>2.3611549768517968</v>
+        <v>-15.456597397157301</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.1216482784096584</v>
+        <v>0.90903224372922864</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.55046764176570662</v>
+        <v>-20.831180096484935</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>9.8962246800289506</v>
+        <v>3.1911752454164315</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>-22.597875009179951</v>
+        <v>-11.110120615115394</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.25192327251759039</v>
+        <v>22.599395387752025</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>-24.638971537257191</v>
+        <v>21.611586003728142</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>10.974904421690198</v>
+        <v>7.8434355183395041</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>21.883677105218908</v>
+        <v>-12.076676675077385</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.59873734051835115</v>
+        <v>-15.476071643181577</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.3112834617432334</v>
+        <v>-3.8945562107835663</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>13.633618378339314</v>
+        <v>-4.945939715580149</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>15.616009637874008</v>
+        <v>13.678014869953984</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>-10.07807569923671</v>
+        <v>-3.4983654305467446</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.40390241230432622</v>
+        <v>20.847241701956605</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.7827015175615735</v>
+        <v>-4.9320062898363979</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>-15.087754640019341</v>
+        <v>15.012988585174959</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>20.308515303992834</v>
+        <v>-4.6585169600929994</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" ca="1" si="1"/>
-        <v>11.187407015705013</v>
+        <v>-17.56823940403947</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>-19.970455274965673</v>
+        <v>-3.5909602529457203</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>-10.265312016366718</v>
+        <v>-17.600192561821089</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>-22.210065028165605</v>
+        <v>22.521639147602571</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>-12.078386564319343</v>
+        <v>-24.559200849205364</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>13.474153104316031</v>
+        <v>23.945960302600852</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>21.358273763538008</v>
+        <v>15.474991645231576</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="0"/>
-        <v>-22.832464406020307</v>
+        <v>12.629447207520741</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ca="1" si="1"/>
-        <v>12.894055998524443</v>
+        <v>-18.802340871955348</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>-16.372213259971417</v>
+        <v>3.2572954157542071</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>-9.3560430665961931</v>
+        <v>23.202473673858762</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>12.614075211877648</v>
+        <v>19.555157352588026</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.9276326737076914</v>
+        <v>-9.5217391232253252</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>-12.452864082671805</v>
+        <v>-11.170901025500457</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>-14.543239471548535</v>
+        <v>-6.4934616329501864</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.6026693229341902</v>
+        <v>16.759444289574205</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="1"/>
-        <v>7.4977413100313655</v>
+        <v>8.8820484393152626</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>23.156821843303739</v>
+        <v>8.9308148114204329</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>15.790709459011488</v>
+        <v>-1.6284231091119423</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>-10.250906350475663</v>
+        <v>-18.856555563713613</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.60894569670779575</v>
+        <v>-17.440294316573873</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>-12.601601752964275</v>
+        <v>1.5836421260011768</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.8490922916796713</v>
+        <v>-9.4404238072912818</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="0"/>
-        <v>6.2832617879587538</v>
+        <v>-2.1199977744661425</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="1"/>
-        <v>-20.49039808709756</v>
+        <v>-14.230260210109098</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>-8.4313691956136267</v>
+        <v>9.7198453513902976</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>9.2189422542803641</v>
+        <v>-24.644957506389325</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>3.3500934898948103</v>
+        <v>-5.7376426504777598</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>-20.465101471110724</v>
+        <v>-23.842949730734709</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>-19.798622286077041</v>
+        <v>5.627673750973571</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>6.9119708661497512</v>
+        <v>17.799624034851583</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="0"/>
-        <v>10.761701829961289</v>
+        <v>-6.7469878823978604</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="1"/>
-        <v>23.917915993592779</v>
+        <v>15.75839840244668</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>3.0367263578057191</v>
+        <v>12.633908850119489</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>4.0902243254134873</v>
+        <v>-5.3688619685807311</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>-18.906673679333032</v>
+        <v>-9.7050383302243919</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>-21.70029313794312</v>
+        <v>-15.31508172324607</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>-10.691198116211092</v>
+        <v>21.967428096920997</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>4.625876299505304</v>
+        <v>-13.084507269318246</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="0"/>
-        <v>-23.770159692265981</v>
+        <v>11.29777465223755</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="1"/>
-        <v>10.399006415857173</v>
+        <v>17.851804111695976</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.4367114459658339</v>
+        <v>4.456426046516178</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.125562577205713</v>
+        <v>1.6802954819682299</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>-8.5281955674495045</v>
+        <v>23.70603214373331</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>14.775354727964626</v>
+        <v>-2.5202989432780996</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>9.7306501519790061</v>
+        <v>-18.002431884356866</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>-10.62574730054941</v>
+        <v>19.759572067151943</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="0"/>
-        <v>19.937990090458037</v>
+        <v>16.860175545313346</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="1"/>
-        <v>-19.210910468789933</v>
+        <v>-16.572578893356372</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9528536890734323</v>
+        <v>-3.5769415736743149</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.1837476182416964</v>
+        <v>23.747938731119845</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>6.2496992507422071</v>
+        <v>-3.4623827947082084</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>-17.673307352897883</v>
+        <v>-10.937841931839326</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>-18.39704369226537</v>
+        <v>-6.7273821911982061</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
-        <v>-11.18295019277944</v>
+        <v>7.4853085746371448</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="0"/>
-        <v>4.0688068577458942</v>
+        <v>13.842852233129584</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="1"/>
-        <v>-15.617535840376256</v>
+        <v>-5.3053184891787843</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>6.3952504303532329</v>
+        <v>7.143994587031635</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>18.84427152938374</v>
+        <v>-9.2197055769595693</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.91110895006227821</v>
+        <v>19.533521864270867</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>-9.3436332380905096</v>
+        <v>-16.155339435704203</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="1"/>
-        <v>-18.786574195632134</v>
+        <v>6.4608505168768708</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="1"/>
-        <v>4.9466293591881936</v>
+        <v>9.5139466026236903</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
-        <v>-14.036105700858641</v>
+        <v>0.17135825894060019</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="1"/>
-        <v>7.3555145930263919</v>
+        <v>4.3587574367307482</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="1"/>
-        <v>2.1383574388828421</v>
+        <v>7.4357285385670409</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>14.155753973478753</v>
+        <v>-6.2199341305115396</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.5381761914509973</v>
+        <v>17.164759688840689</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>-9.3725194843343793</v>
+        <v>2.8374743484255021</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="1"/>
-        <v>-22.764346387159517</v>
+        <v>0.20815913286601884</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="1"/>
-        <v>-22.237195615054372</v>
+        <v>19.871900310798921</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.425508698034843</v>
+        <v>16.422698248023778</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="1"/>
-        <v>5.0027586010391936</v>
+        <v>-14.748252707283738</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="1"/>
-        <v>-13.786338236472545</v>
+        <v>-20.281092150452796</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.34452333476871644</v>
+        <v>-20.712474602632668</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>-10.839631458316484</v>
+        <v>-24.500830014176138</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>13.74239491328251</v>
+        <v>-14.910786769980543</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="1"/>
-        <v>18.181388748681584</v>
+        <v>-14.089763791667725</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.8933200144314561</v>
+        <v>-4.7953221677784157</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.0514254868567434</v>
+        <v>-19.526572675496102</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" ca="1" si="1"/>
-        <v>18.453838815889192</v>
+        <v>5.9280741474604284</v>
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="1"/>
-        <v>-20.328270057506053</v>
+        <v>-18.331052156958215</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>-14.021109606975784</v>
+        <v>14.524274216968109</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="1"/>
-        <v>5.9683031208309245</v>
+        <v>-0.99572800941875172</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="1"/>
-        <v>23.02123816722024</v>
+        <v>-11.347805911566821</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="1"/>
-        <v>-17.508975645463948</v>
+        <v>-24.54221857329188</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="1"/>
-        <v>-9.3041542065536778</v>
+        <v>22.386719567185452</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="1"/>
-        <v>8.8953730363327423</v>
+        <v>-10.603556347833143</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.1654179804155973</v>
+        <v>-3.4449184743120327</v>
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="1"/>
-        <v>-8.30477950201821</v>
+        <v>14.027872320926335</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>-11.129292808279361</v>
+        <v>8.2020915522425923</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="1"/>
-        <v>4.6910812773576396</v>
+        <v>17.63823074729526</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.8172402094832734</v>
+        <v>11.461514940824728</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="1"/>
-        <v>24.51966803448736</v>
+        <v>8.2747431896358137</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="1"/>
-        <v>18.828980491302502</v>
+        <v>-18.287256798037138</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="1"/>
-        <v>-24.180543454715696</v>
+        <v>-7.8051399379536477</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" ca="1" si="1"/>
-        <v>-24.710883598093712</v>
+        <v>-11.727564332582524</v>
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="1"/>
-        <v>-9.9305745108070553</v>
+        <v>-7.0894793875962705</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>7.3700014957105253</v>
+        <v>-4.8741853696370576</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.134981560745441</v>
+        <v>-22.543351547353517</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="1"/>
-        <v>-22.378279138546169</v>
+        <v>22.967487567521232</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="1"/>
-        <v>-16.898773919174793</v>
+        <v>-4.9732288604205195</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="1"/>
-        <v>11.602317477380495</v>
+        <v>11.005466843868447</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="1"/>
-        <v>4.5511821900642282</v>
+        <v>0.70947361782899776</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.78201180443408091</v>
+        <v>17.819675247261493</v>
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="1"/>
-        <v>-17.217330982361002</v>
+        <v>12.024257439937962</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>-24.814866342242642</v>
+        <v>20.642452631347965</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="1"/>
-        <v>5.3797395481790176</v>
+        <v>-24.356321884045368</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="1"/>
-        <v>5.1876575340398787</v>
+        <v>17.955198620364989</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="1"/>
-        <v>-23.920960217110377</v>
+        <v>15.276095650766813</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="1"/>
-        <v>-7.9604214049762412</v>
+        <v>-10.289815578052769</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.9357013268077097</v>
+        <v>13.52347418655286</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.1460208332445632</v>
+        <v>23.420011031917618</v>
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="1"/>
-        <v>7.8603884746392083</v>
+        <v>11.522644088847208</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>24.916714454529085</v>
+        <v>3.853224841774928</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="1"/>
-        <v>-18.496844129879758</v>
+        <v>-10.596579696826335</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="1"/>
-        <v>-15.393096480746877</v>
+        <v>3.4439973495490435</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="1"/>
-        <v>16.007629970694772</v>
+        <v>9.0909718587386408</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="1"/>
-        <v>12.452601978697196</v>
+        <v>-13.264648091296211</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="1"/>
-        <v>1.4359496114216377</v>
+        <v>23.502356469382939</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" ca="1" si="1"/>
-        <v>10.899447782632386</v>
+        <v>-3.7862336117031674</v>
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="1"/>
-        <v>13.553125419344347</v>
+        <v>-8.0832292444072067</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>2.8914719092622043</v>
+        <v>-20.963247485146415</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="1"/>
-        <v>-18.652340681629969</v>
+        <v>-19.579887741518604</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.6719593199127942</v>
+        <v>4.1553867756483278</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="1"/>
-        <v>19.453731555757251</v>
+        <v>-11.246058727817054</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="1"/>
-        <v>6.0433988320784131</v>
+        <v>-3.9944901980756882</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="1"/>
-        <v>7.5411352669249325</v>
+        <v>2.8270056155549845</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" ca="1" si="1"/>
-        <v>17.355640758389981</v>
+        <v>-8.9797967922223236</v>
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="1"/>
-        <v>-14.294209855858043</v>
+        <v>12.648987894713521</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0968163206004284</v>
+        <v>10.459408338299106</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="1"/>
-        <v>-15.928698996786805</v>
+        <v>9.8428982485787273</v>
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.53905862789265058</v>
+        <v>20.61106745891869</v>
       </c>
       <c r="F26">
         <f t="shared" ca="1" si="1"/>
-        <v>-8.6954480380737884</v>
+        <v>17.017540407904448</v>
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="1"/>
-        <v>9.8806943822486204</v>
+        <v>7.7149550285913335</v>
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.36206631570309611</v>
+        <v>-0.26334765207963784</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" ca="1" si="1"/>
-        <v>21.68822553967793</v>
+        <v>20.758832504649845</v>
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="1"/>
-        <v>-10.758428889038946</v>
+        <v>15.740849666976757</v>
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="1"/>
-        <v>-19.460680162324898</v>
+        <v>-23.784932583341455</v>
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="1"/>
-        <v>7.8761460843179734</v>
+        <v>23.870938377176671</v>
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2728096830230413</v>
+        <v>-12.44760533338617</v>
       </c>
       <c r="F27">
         <f t="shared" ca="1" si="1"/>
-        <v>12.345890351938266</v>
+        <v>5.0128258946799846</v>
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="1"/>
-        <v>-9.6425509279758188</v>
+        <v>-9.0298216004831726</v>
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="1"/>
-        <v>3.4200008176665513</v>
+        <v>8.6853507078524927</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.21940478253296192</v>
+        <v>1.8729419530878033</v>
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="1"/>
-        <v>1.8207009752453764</v>
+        <v>-23.419289107134773</v>
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="1"/>
-        <v>5.1647220457809624</v>
+        <v>14.929938944018133</v>
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="1"/>
-        <v>-8.0053394983474426</v>
+        <v>-10.557948733065164</v>
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="1"/>
-        <v>-11.651941175656304</v>
+        <v>-14.352588445585473</v>
       </c>
       <c r="F28">
         <f t="shared" ca="1" si="1"/>
-        <v>8.6379867351335875</v>
+        <v>-19.848948872362715</v>
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="1"/>
-        <v>-15.707519494954713</v>
+        <v>3.0332046205115368</v>
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="1"/>
-        <v>21.976118061848155</v>
+        <v>24.481097515154367</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" ca="1" si="1"/>
-        <v>-9.5097683368564994</v>
+        <v>14.068147496572294</v>
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="1"/>
-        <v>11.159946220912495</v>
+        <v>-2.4566079744489109</v>
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="1"/>
-        <v>18.304403730818272</v>
+        <v>-13.280704023705459</v>
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="1"/>
-        <v>5.764131101201297</v>
+        <v>4.2100591453716127</v>
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="1"/>
-        <v>-9.9972879908689478</v>
+        <v>16.86454710896912</v>
       </c>
       <c r="F29">
         <f t="shared" ca="1" si="1"/>
-        <v>20.294436187052433</v>
+        <v>-10.091954974611806</v>
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="1"/>
-        <v>16.671208838991838</v>
+        <v>-23.789124062239704</v>
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="1"/>
-        <v>0.66085585806158775</v>
+        <v>-17.904111884312446</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" ca="1" si="1"/>
-        <v>-17.5910337111915</v>
+        <v>-2.9943513198018756</v>
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="1"/>
-        <v>17.783343346055155</v>
+        <v>-1.8191852581504477</v>
       </c>
       <c r="C30">
         <f t="shared" ca="1" si="1"/>
-        <v>2.0867979411518185</v>
+        <v>15.30493311002315</v>
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.9449708184065919</v>
+        <v>22.433559056412165</v>
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="1"/>
-        <v>8.8967501025623079</v>
+        <v>5.042363283662155</v>
       </c>
       <c r="F30">
         <f t="shared" ca="1" si="1"/>
-        <v>-23.010447636858629</v>
+        <v>-19.32029024960071</v>
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="1"/>
-        <v>16.728571097256605</v>
+        <v>-24.385262891388887</v>
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.905012082540285</v>
+        <v>-23.027463431881301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>